<commit_message>
regional de Amilkar Quezo
</commit_message>
<xml_diff>
--- a/Nomina.xlsx
+++ b/Nomina.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\Udabol-SistemasDeInformacionYSistemasInteligentes\UDABOL_202202\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BB39B4-FA84-4FE5-B24D-8109D008C8B7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Hoja1"/>
-    <sheet r:id="rId2" sheetId="2" name="Hoja2"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="430">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -1302,14 +1308,16 @@
   </si>
   <si>
     <t>CI:8257209</t>
+  </si>
+  <si>
+    <t>La Paz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1392,61 +1400,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1457,10 +1458,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1498,71 +1499,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1590,7 +1591,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -1613,11 +1614,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -1626,13 +1627,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1642,7 +1643,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1651,7 +1652,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1660,7 +1661,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1668,10 +1669,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1736,7 +1737,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1744,17 +1745,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="12.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="13.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="13.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1">
       <c r="A1" s="9">
         <v>1</v>
       </c>
@@ -1772,7 +1771,7 @@
         <v>9845916</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:6" ht="18.75" customHeight="1">
       <c r="A2" s="9">
         <v>2</v>
       </c>
@@ -1792,7 +1791,7 @@
         <v>4308676</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:6" ht="18.75" customHeight="1">
       <c r="A3" s="9">
         <v>3</v>
       </c>
@@ -1812,7 +1811,7 @@
         <v>5273148</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:6" ht="18.75" customHeight="1">
       <c r="A4" s="9">
         <v>4</v>
       </c>
@@ -1832,7 +1831,7 @@
         <v>10680663</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:6" ht="18.75" customHeight="1">
       <c r="A5" s="9">
         <v>5</v>
       </c>
@@ -1852,7 +1851,7 @@
         <v>12873339</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:6" ht="18.75" customHeight="1">
       <c r="A6" s="9">
         <v>6</v>
       </c>
@@ -1872,7 +1871,7 @@
         <v>7351544</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:6" ht="18.75" customHeight="1">
       <c r="A7" s="9">
         <v>7</v>
       </c>
@@ -1892,7 +1891,7 @@
         <v>7296889</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:6" ht="18.75" customHeight="1">
       <c r="A8" s="9">
         <v>8</v>
       </c>
@@ -1912,7 +1911,7 @@
         <v>9083846</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:6" ht="18.75" customHeight="1">
       <c r="A9" s="9">
         <v>9</v>
       </c>
@@ -1930,7 +1929,7 @@
         <v>8437859</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:6" ht="18.75" customHeight="1">
       <c r="A10" s="9">
         <v>10</v>
       </c>
@@ -1950,7 +1949,7 @@
         <v>11304597</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:6" ht="18.75" customHeight="1">
       <c r="A11" s="9">
         <v>11</v>
       </c>
@@ -1968,7 +1967,7 @@
         <v>8911045</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:6" ht="18.75" customHeight="1">
       <c r="A12" s="9">
         <v>12</v>
       </c>
@@ -1986,7 +1985,7 @@
         <v>6717766</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:6" ht="18.75" customHeight="1">
       <c r="A13" s="9">
         <v>13</v>
       </c>
@@ -2006,7 +2005,7 @@
         <v>2631732</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:6" ht="18.75" customHeight="1">
       <c r="A14" s="9">
         <v>14</v>
       </c>
@@ -2024,7 +2023,7 @@
       </c>
       <c r="F14" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:6" ht="18.75" customHeight="1">
       <c r="A15" s="9">
         <v>15</v>
       </c>
@@ -2044,7 +2043,7 @@
         <v>33970</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:6" ht="18.75" customHeight="1">
       <c r="A16" s="9">
         <v>16</v>
       </c>
@@ -2064,7 +2063,7 @@
         <v>9899773</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:6" ht="18.75" customHeight="1">
       <c r="A17" s="9">
         <v>17</v>
       </c>
@@ -2084,7 +2083,7 @@
         <v>7041610</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:6" ht="18.75" customHeight="1">
       <c r="A18" s="9">
         <v>18</v>
       </c>
@@ -2104,7 +2103,7 @@
         <v>12669252</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:6" ht="18.75" customHeight="1">
       <c r="A19" s="9">
         <v>19</v>
       </c>
@@ -2124,7 +2123,7 @@
         <v>10931935</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:6" ht="18.75" customHeight="1">
       <c r="A20" s="9">
         <v>20</v>
       </c>
@@ -2144,7 +2143,7 @@
         <v>6920030</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:6" ht="18.75" customHeight="1">
       <c r="A21" s="9">
         <v>21</v>
       </c>
@@ -2164,7 +2163,7 @@
         <v>6434495</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row r="22" spans="1:6" ht="18.75" customHeight="1">
       <c r="A22" s="9">
         <v>22</v>
       </c>
@@ -2184,7 +2183,7 @@
         <v>9155549</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row r="23" spans="1:6" ht="18.75" customHeight="1">
       <c r="A23" s="9">
         <v>23</v>
       </c>
@@ -2202,7 +2201,7 @@
         <v>6823974</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row r="24" spans="1:6" ht="18.75" customHeight="1">
       <c r="A24" s="9">
         <v>24</v>
       </c>
@@ -2222,7 +2221,7 @@
         <v>2622061</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row r="25" spans="1:6" ht="18.75" customHeight="1">
       <c r="A25" s="9">
         <v>25</v>
       </c>
@@ -2240,7 +2239,7 @@
         <v>7838112</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row r="26" spans="1:6" ht="18.75" customHeight="1">
       <c r="A26" s="9">
         <v>26</v>
       </c>
@@ -2260,7 +2259,7 @@
         <v>12864046</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row r="27" spans="1:6" ht="18.75" customHeight="1">
       <c r="A27" s="9">
         <v>27</v>
       </c>
@@ -2280,7 +2279,7 @@
         <v>9110161</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row r="28" spans="1:6" ht="18.75" customHeight="1">
       <c r="A28" s="9">
         <v>28</v>
       </c>
@@ -2296,7 +2295,7 @@
         <v>9911855</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row r="29" spans="1:6" ht="18.75" customHeight="1">
       <c r="A29" s="9">
         <v>29</v>
       </c>
@@ -2314,7 +2313,7 @@
         <v>9459513</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row r="30" spans="1:6" ht="18.75" customHeight="1">
       <c r="A30" s="9">
         <v>30</v>
       </c>
@@ -2332,7 +2331,7 @@
         <v>10954950</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row r="31" spans="1:6" ht="18.75" customHeight="1">
       <c r="A31" s="9">
         <v>31</v>
       </c>
@@ -2350,7 +2349,7 @@
         <v>8028972</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row r="32" spans="1:6" ht="18.75" customHeight="1">
       <c r="A32" s="9">
         <v>32</v>
       </c>
@@ -2370,7 +2369,7 @@
         <v>428</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row r="33" spans="1:6" ht="18.75" customHeight="1">
       <c r="A33" s="9">
         <v>33</v>
       </c>
@@ -2396,36 +2395,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:Q151"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="G42" workbookViewId="0">
+      <selection activeCell="L46" sqref="L46"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="31.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="9.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="9.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="15.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="30.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="22.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="37.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="8" width="43.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="8" width="37.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="8" width="27.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="8" width="27.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="13" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="27.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="13.5546875" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:17" ht="18.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2468,9 +2464,9 @@
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:17" ht="18.75" customHeight="1">
       <c r="A2" s="4">
-        <v>44816.89942129629</v>
+        <v>44816.899421296293</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>12</v>
@@ -2509,7 +2505,7 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:17" ht="18.75" customHeight="1">
       <c r="A3" s="4">
         <v>44816.899618055555</v>
       </c>
@@ -2550,7 +2546,7 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:17" ht="18.75" customHeight="1">
       <c r="A4" s="4">
         <v>44816.90053240741</v>
       </c>
@@ -2591,7 +2587,7 @@
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:17" ht="18.75" customHeight="1">
       <c r="A5" s="4">
         <v>44816.90079861111</v>
       </c>
@@ -2632,7 +2628,7 @@
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:17" ht="18.75" customHeight="1">
       <c r="A6" s="4">
         <v>44816.90079861111</v>
       </c>
@@ -2673,7 +2669,7 @@
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:17" ht="18.75" customHeight="1">
       <c r="A7" s="4">
         <v>44816.900821759256</v>
       </c>
@@ -2714,9 +2710,9 @@
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:17" ht="18.75" customHeight="1">
       <c r="A8" s="4">
-        <v>44816.90090277778</v>
+        <v>44816.900902777779</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>54</v>
@@ -2755,7 +2751,7 @@
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:17" ht="18.75" customHeight="1">
       <c r="A9" s="4">
         <v>44816.900972222225</v>
       </c>
@@ -2796,9 +2792,9 @@
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:17" ht="18.75" customHeight="1">
       <c r="A10" s="4">
-        <v>44816.90136574074</v>
+        <v>44816.901365740741</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>69</v>
@@ -2837,9 +2833,9 @@
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:17" ht="18.75" customHeight="1">
       <c r="A11" s="4">
-        <v>44816.90200231481</v>
+        <v>44816.902002314811</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>76</v>
@@ -2878,9 +2874,9 @@
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:17" ht="18.75" customHeight="1">
       <c r="A12" s="4">
-        <v>44816.90200231481</v>
+        <v>44816.902002314811</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>82</v>
@@ -2919,9 +2915,9 @@
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:17" ht="18.75" customHeight="1">
       <c r="A13" s="4">
-        <v>44816.90210648148</v>
+        <v>44816.902106481481</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>90</v>
@@ -2960,9 +2956,9 @@
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:17" ht="18.75" customHeight="1">
       <c r="A14" s="4">
-        <v>44816.90212962963</v>
+        <v>44816.902129629627</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>98</v>
@@ -3001,7 +2997,7 @@
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:17" ht="18.75" customHeight="1">
       <c r="A15" s="4">
         <v>44816.902141203704</v>
       </c>
@@ -3042,9 +3038,9 @@
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:17" ht="18.75" customHeight="1">
       <c r="A16" s="4">
-        <v>44816.90219907407</v>
+        <v>44816.902199074073</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>113</v>
@@ -3083,9 +3079,9 @@
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:17" ht="18.75" customHeight="1">
       <c r="A17" s="4">
-        <v>44816.90324074074</v>
+        <v>44816.903240740743</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>120</v>
@@ -3124,9 +3120,9 @@
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:17" ht="18.75" customHeight="1">
       <c r="A18" s="4">
-        <v>44816.90335648148</v>
+        <v>44816.903356481482</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>127</v>
@@ -3165,7 +3161,7 @@
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:17" ht="18.75" customHeight="1">
       <c r="A19" s="4">
         <v>44816.903657407405</v>
       </c>
@@ -3206,9 +3202,9 @@
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:17" ht="18.75" customHeight="1">
       <c r="A20" s="4">
-        <v>44816.90369212963</v>
+        <v>44816.903692129628</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>142</v>
@@ -3247,9 +3243,9 @@
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:17" ht="18.75" customHeight="1">
       <c r="A21" s="4">
-        <v>44816.90385416667</v>
+        <v>44816.903854166667</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>149</v>
@@ -3288,9 +3284,9 @@
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row r="22" spans="1:17" ht="18.75" customHeight="1">
       <c r="A22" s="4">
-        <v>44816.90443287037</v>
+        <v>44816.904432870368</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>155</v>
@@ -3329,9 +3325,9 @@
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row r="23" spans="1:17" ht="18.75" customHeight="1">
       <c r="A23" s="4">
-        <v>44816.90445601852</v>
+        <v>44816.904456018521</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>162</v>
@@ -3370,9 +3366,9 @@
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row r="24" spans="1:17" ht="18.75" customHeight="1">
       <c r="A24" s="4">
-        <v>44816.90460648148</v>
+        <v>44816.904606481483</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>168</v>
@@ -3411,9 +3407,9 @@
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row r="25" spans="1:17" ht="18.75" customHeight="1">
       <c r="A25" s="4">
-        <v>44816.9047337963</v>
+        <v>44816.904733796298</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>176</v>
@@ -3452,9 +3448,9 @@
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row r="26" spans="1:17" ht="18.75" customHeight="1">
       <c r="A26" s="4">
-        <v>44816.90489583334</v>
+        <v>44816.904895833337</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>183</v>
@@ -3493,9 +3489,9 @@
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row r="27" spans="1:17" ht="18.75" customHeight="1">
       <c r="A27" s="4">
-        <v>44816.90553240741</v>
+        <v>44816.905532407407</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>190</v>
@@ -3534,9 +3530,9 @@
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row r="28" spans="1:17" ht="18.75" customHeight="1">
       <c r="A28" s="4">
-        <v>44816.90611111111</v>
+        <v>44816.906111111108</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>197</v>
@@ -3575,7 +3571,7 @@
       <c r="P28" s="3"/>
       <c r="Q28" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row r="29" spans="1:17" ht="18.75" customHeight="1">
       <c r="A29" s="4">
         <v>44816.906689814816</v>
       </c>
@@ -3616,9 +3612,9 @@
       <c r="P29" s="3"/>
       <c r="Q29" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row r="30" spans="1:17" ht="18.75" customHeight="1">
       <c r="A30" s="4">
-        <v>44816.90688657408</v>
+        <v>44816.906886574077</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>212</v>
@@ -3657,9 +3653,9 @@
       <c r="P30" s="3"/>
       <c r="Q30" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row r="31" spans="1:17" ht="18.75" customHeight="1">
       <c r="A31" s="4">
-        <v>44816.90694444445</v>
+        <v>44816.906944444447</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>218</v>
@@ -3698,9 +3694,9 @@
       <c r="P31" s="3"/>
       <c r="Q31" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row r="32" spans="1:17" ht="18.75" customHeight="1">
       <c r="A32" s="4">
-        <v>44816.90813657407</v>
+        <v>44816.908136574071</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>226</v>
@@ -3739,9 +3735,9 @@
       <c r="P32" s="3"/>
       <c r="Q32" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row r="33" spans="1:17" ht="18.75" customHeight="1">
       <c r="A33" s="4">
-        <v>44816.90820601852</v>
+        <v>44816.908206018517</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>233</v>
@@ -3780,7 +3776,7 @@
       <c r="P33" s="3"/>
       <c r="Q33" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row r="34" spans="1:17" ht="18.75" customHeight="1">
       <c r="A34" s="4">
         <v>44816.908321759256</v>
       </c>
@@ -3821,7 +3817,7 @@
       <c r="P34" s="3"/>
       <c r="Q34" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    <row r="35" spans="1:17" ht="18.75" customHeight="1">
       <c r="A35" s="4">
         <v>44816.909525462965</v>
       </c>
@@ -3862,7 +3858,7 @@
       <c r="P35" s="3"/>
       <c r="Q35" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row r="36" spans="1:17" ht="18.75" customHeight="1">
       <c r="A36" s="4">
         <v>44816.909907407404</v>
       </c>
@@ -3903,9 +3899,9 @@
       <c r="P36" s="3"/>
       <c r="Q36" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+    <row r="37" spans="1:17" ht="18.75" customHeight="1">
       <c r="A37" s="4">
-        <v>44816.92482638889</v>
+        <v>44816.924826388888</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>262</v>
@@ -3944,7 +3940,7 @@
       <c r="P37" s="3"/>
       <c r="Q37" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+    <row r="38" spans="1:17" ht="18.75" customHeight="1">
       <c r="A38" s="4">
         <v>44816.93582175926</v>
       </c>
@@ -3985,9 +3981,9 @@
       <c r="P38" s="3"/>
       <c r="Q38" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+    <row r="39" spans="1:17" ht="18.75" customHeight="1">
       <c r="A39" s="4">
-        <v>44817.34590277778</v>
+        <v>44817.345902777779</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>276</v>
@@ -4026,9 +4022,9 @@
       <c r="P39" s="3"/>
       <c r="Q39" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row r="40" spans="1:17" ht="18.75" customHeight="1">
       <c r="A40" s="4">
-        <v>44817.72846064815</v>
+        <v>44817.728460648148</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>283</v>
@@ -4069,9 +4065,9 @@
       <c r="P40" s="3"/>
       <c r="Q40" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+    <row r="41" spans="1:17" ht="18.75" customHeight="1">
       <c r="A41" s="4">
-        <v>44817.85704861111</v>
+        <v>44817.857048611113</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>292</v>
@@ -4110,9 +4106,9 @@
       <c r="P41" s="3"/>
       <c r="Q41" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+    <row r="42" spans="1:17" ht="18.75" customHeight="1">
       <c r="A42" s="4">
-        <v>44817.97329861111</v>
+        <v>44817.973298611112</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>299</v>
@@ -4151,9 +4147,9 @@
       <c r="P42" s="3"/>
       <c r="Q42" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+    <row r="43" spans="1:17" ht="18.75" customHeight="1">
       <c r="A43" s="4">
-        <v>44818.01280092593</v>
+        <v>44818.012800925928</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>305</v>
@@ -4192,7 +4188,7 @@
       <c r="P43" s="3"/>
       <c r="Q43" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+    <row r="44" spans="1:17" ht="18.75" customHeight="1">
       <c r="A44" s="4">
         <v>44818.452256944445</v>
       </c>
@@ -4233,9 +4229,9 @@
       <c r="P44" s="3"/>
       <c r="Q44" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+    <row r="45" spans="1:17" ht="18.75" customHeight="1">
       <c r="A45" s="4">
-        <v>44818.5594212963</v>
+        <v>44818.559421296297</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>319</v>
@@ -4274,7 +4270,7 @@
       <c r="P45" s="3"/>
       <c r="Q45" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+    <row r="46" spans="1:17" ht="18.75" customHeight="1">
       <c r="A46" s="4">
         <v>44818.81627314815</v>
       </c>
@@ -4308,16 +4304,18 @@
       <c r="K46" s="5" t="s">
         <v>332</v>
       </c>
-      <c r="L46" s="5"/>
+      <c r="L46" s="5" t="s">
+        <v>429</v>
+      </c>
       <c r="M46" s="3"/>
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
       <c r="Q46" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+    <row r="47" spans="1:17" ht="18.75" customHeight="1">
       <c r="A47" s="4">
-        <v>44818.83111111111</v>
+        <v>44818.831111111111</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>333</v>
@@ -4356,9 +4354,9 @@
       <c r="P47" s="3"/>
       <c r="Q47" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+    <row r="48" spans="1:17" ht="18.75" customHeight="1">
       <c r="A48" s="4">
-        <v>44819.45891203704</v>
+        <v>44819.458912037036</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>340</v>
@@ -4397,9 +4395,9 @@
       <c r="P48" s="3"/>
       <c r="Q48" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
+    <row r="49" spans="1:17" ht="18.75" customHeight="1">
       <c r="A49" s="4">
-        <v>44819.79439814815</v>
+        <v>44819.794398148151</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>346</v>
@@ -4438,9 +4436,9 @@
       <c r="P49" s="3"/>
       <c r="Q49" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+    <row r="50" spans="1:17" ht="18.75" customHeight="1">
       <c r="A50" s="4">
-        <v>44819.81234953704</v>
+        <v>44819.812349537038</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>353</v>
@@ -4479,7 +4477,7 @@
       <c r="P50" s="3"/>
       <c r="Q50" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
+    <row r="51" spans="1:17" ht="18.75" customHeight="1">
       <c r="A51" s="4">
         <v>44819.851585648146</v>
       </c>
@@ -4520,7 +4518,7 @@
       <c r="P51" s="3"/>
       <c r="Q51" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
+    <row r="52" spans="1:17" ht="18.75" customHeight="1">
       <c r="A52" s="6"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -4539,7 +4537,7 @@
       <c r="P52" s="3"/>
       <c r="Q52" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
+    <row r="53" spans="1:17" ht="18.75" customHeight="1">
       <c r="A53" s="6"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -4558,7 +4556,7 @@
       <c r="P53" s="3"/>
       <c r="Q53" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
+    <row r="54" spans="1:17" ht="18.75" customHeight="1">
       <c r="A54" s="6"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -4577,7 +4575,7 @@
       <c r="P54" s="3"/>
       <c r="Q54" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
+    <row r="55" spans="1:17" ht="18.75" customHeight="1">
       <c r="A55" s="6"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -4596,7 +4594,7 @@
       <c r="P55" s="3"/>
       <c r="Q55" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
+    <row r="56" spans="1:17" ht="18.75" customHeight="1">
       <c r="A56" s="6"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -4615,7 +4613,7 @@
       <c r="P56" s="3"/>
       <c r="Q56" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
+    <row r="57" spans="1:17" ht="18.75" customHeight="1">
       <c r="A57" s="6"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -4634,7 +4632,7 @@
       <c r="P57" s="3"/>
       <c r="Q57" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
+    <row r="58" spans="1:17" ht="18.75" customHeight="1">
       <c r="A58" s="6"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -4653,7 +4651,7 @@
       <c r="P58" s="3"/>
       <c r="Q58" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
+    <row r="59" spans="1:17" ht="18.75" customHeight="1">
       <c r="A59" s="6"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -4672,7 +4670,7 @@
       <c r="P59" s="3"/>
       <c r="Q59" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
+    <row r="60" spans="1:17" ht="18.75" customHeight="1">
       <c r="A60" s="6"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -4691,7 +4689,7 @@
       <c r="P60" s="3"/>
       <c r="Q60" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
+    <row r="61" spans="1:17" ht="18.75" customHeight="1">
       <c r="A61" s="6"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -4710,7 +4708,7 @@
       <c r="P61" s="3"/>
       <c r="Q61" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
+    <row r="62" spans="1:17" ht="18.75" customHeight="1">
       <c r="A62" s="6"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -4729,7 +4727,7 @@
       <c r="P62" s="3"/>
       <c r="Q62" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
+    <row r="63" spans="1:17" ht="18.75" customHeight="1">
       <c r="A63" s="6"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -4748,7 +4746,7 @@
       <c r="P63" s="3"/>
       <c r="Q63" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
+    <row r="64" spans="1:17" ht="18.75" customHeight="1">
       <c r="A64" s="6"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -4767,7 +4765,7 @@
       <c r="P64" s="3"/>
       <c r="Q64" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
+    <row r="65" spans="1:17" ht="18.75" customHeight="1">
       <c r="A65" s="6"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -4786,7 +4784,7 @@
       <c r="P65" s="3"/>
       <c r="Q65" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
+    <row r="66" spans="1:17" ht="18.75" customHeight="1">
       <c r="A66" s="6"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -4805,7 +4803,7 @@
       <c r="P66" s="3"/>
       <c r="Q66" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
+    <row r="67" spans="1:17" ht="18.75" customHeight="1">
       <c r="A67" s="6"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -4824,7 +4822,7 @@
       <c r="P67" s="3"/>
       <c r="Q67" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
+    <row r="68" spans="1:17" ht="18.75" customHeight="1">
       <c r="A68" s="6"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -4843,7 +4841,7 @@
       <c r="P68" s="3"/>
       <c r="Q68" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
+    <row r="69" spans="1:17" ht="18.75" customHeight="1">
       <c r="A69" s="6"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -4862,7 +4860,7 @@
       <c r="P69" s="3"/>
       <c r="Q69" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
+    <row r="70" spans="1:17" ht="18.75" customHeight="1">
       <c r="A70" s="6"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -4881,7 +4879,7 @@
       <c r="P70" s="3"/>
       <c r="Q70" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
+    <row r="71" spans="1:17" ht="18.75" customHeight="1">
       <c r="A71" s="6"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -4900,7 +4898,7 @@
       <c r="P71" s="3"/>
       <c r="Q71" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
+    <row r="72" spans="1:17" ht="18.75" customHeight="1">
       <c r="A72" s="6"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -4919,7 +4917,7 @@
       <c r="P72" s="3"/>
       <c r="Q72" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
+    <row r="73" spans="1:17" ht="18.75" customHeight="1">
       <c r="A73" s="6"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -4938,7 +4936,7 @@
       <c r="P73" s="3"/>
       <c r="Q73" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
+    <row r="74" spans="1:17" ht="18.75" customHeight="1">
       <c r="A74" s="6"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -4957,7 +4955,7 @@
       <c r="P74" s="3"/>
       <c r="Q74" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
+    <row r="75" spans="1:17" ht="18.75" customHeight="1">
       <c r="A75" s="6"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -4976,7 +4974,7 @@
       <c r="P75" s="3"/>
       <c r="Q75" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
+    <row r="76" spans="1:17" ht="18.75" customHeight="1">
       <c r="A76" s="6"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -4995,7 +4993,7 @@
       <c r="P76" s="3"/>
       <c r="Q76" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
+    <row r="77" spans="1:17" ht="18.75" customHeight="1">
       <c r="A77" s="6"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -5014,7 +5012,7 @@
       <c r="P77" s="3"/>
       <c r="Q77" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
+    <row r="78" spans="1:17" ht="18.75" customHeight="1">
       <c r="A78" s="6"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -5033,7 +5031,7 @@
       <c r="P78" s="3"/>
       <c r="Q78" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
+    <row r="79" spans="1:17" ht="18.75" customHeight="1">
       <c r="A79" s="6"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -5052,7 +5050,7 @@
       <c r="P79" s="3"/>
       <c r="Q79" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
+    <row r="80" spans="1:17" ht="18.75" customHeight="1">
       <c r="A80" s="6"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -5071,7 +5069,7 @@
       <c r="P80" s="3"/>
       <c r="Q80" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
+    <row r="81" spans="1:17" ht="18.75" customHeight="1">
       <c r="A81" s="6"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -5090,7 +5088,7 @@
       <c r="P81" s="3"/>
       <c r="Q81" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
+    <row r="82" spans="1:17" ht="18.75" customHeight="1">
       <c r="A82" s="6"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
@@ -5109,7 +5107,7 @@
       <c r="P82" s="3"/>
       <c r="Q82" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
+    <row r="83" spans="1:17" ht="18.75" customHeight="1">
       <c r="A83" s="6"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -5128,7 +5126,7 @@
       <c r="P83" s="3"/>
       <c r="Q83" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
+    <row r="84" spans="1:17" ht="18.75" customHeight="1">
       <c r="A84" s="6"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
@@ -5147,7 +5145,7 @@
       <c r="P84" s="3"/>
       <c r="Q84" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
+    <row r="85" spans="1:17" ht="18.75" customHeight="1">
       <c r="A85" s="6"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
@@ -5166,7 +5164,7 @@
       <c r="P85" s="3"/>
       <c r="Q85" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
+    <row r="86" spans="1:17" ht="18.75" customHeight="1">
       <c r="A86" s="6"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
@@ -5185,7 +5183,7 @@
       <c r="P86" s="3"/>
       <c r="Q86" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
+    <row r="87" spans="1:17" ht="18.75" customHeight="1">
       <c r="A87" s="6"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -5204,7 +5202,7 @@
       <c r="P87" s="3"/>
       <c r="Q87" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
+    <row r="88" spans="1:17" ht="18.75" customHeight="1">
       <c r="A88" s="6"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -5223,7 +5221,7 @@
       <c r="P88" s="3"/>
       <c r="Q88" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
+    <row r="89" spans="1:17" ht="18.75" customHeight="1">
       <c r="A89" s="6"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -5242,7 +5240,7 @@
       <c r="P89" s="3"/>
       <c r="Q89" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
+    <row r="90" spans="1:17" ht="18.75" customHeight="1">
       <c r="A90" s="6"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -5261,7 +5259,7 @@
       <c r="P90" s="3"/>
       <c r="Q90" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
+    <row r="91" spans="1:17" ht="18.75" customHeight="1">
       <c r="A91" s="6"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
@@ -5280,7 +5278,7 @@
       <c r="P91" s="3"/>
       <c r="Q91" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
+    <row r="92" spans="1:17" ht="18.75" customHeight="1">
       <c r="A92" s="6"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
@@ -5299,7 +5297,7 @@
       <c r="P92" s="3"/>
       <c r="Q92" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
+    <row r="93" spans="1:17" ht="18.75" customHeight="1">
       <c r="A93" s="6"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
@@ -5318,7 +5316,7 @@
       <c r="P93" s="3"/>
       <c r="Q93" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
+    <row r="94" spans="1:17" ht="18.75" customHeight="1">
       <c r="A94" s="6"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
@@ -5337,7 +5335,7 @@
       <c r="P94" s="3"/>
       <c r="Q94" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
+    <row r="95" spans="1:17" ht="18.75" customHeight="1">
       <c r="A95" s="6"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
@@ -5356,7 +5354,7 @@
       <c r="P95" s="3"/>
       <c r="Q95" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
+    <row r="96" spans="1:17" ht="18.75" customHeight="1">
       <c r="A96" s="6"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
@@ -5375,7 +5373,7 @@
       <c r="P96" s="3"/>
       <c r="Q96" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
+    <row r="97" spans="1:17" ht="18.75" customHeight="1">
       <c r="A97" s="6"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
@@ -5394,7 +5392,7 @@
       <c r="P97" s="3"/>
       <c r="Q97" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
+    <row r="98" spans="1:17" ht="18.75" customHeight="1">
       <c r="A98" s="6"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
@@ -5413,7 +5411,7 @@
       <c r="P98" s="3"/>
       <c r="Q98" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
+    <row r="99" spans="1:17" ht="18.75" customHeight="1">
       <c r="A99" s="6"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
@@ -5432,7 +5430,7 @@
       <c r="P99" s="3"/>
       <c r="Q99" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
+    <row r="100" spans="1:17" ht="18.75" customHeight="1">
       <c r="A100" s="6"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
@@ -5451,7 +5449,7 @@
       <c r="P100" s="3"/>
       <c r="Q100" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
+    <row r="101" spans="1:17" ht="18.75" customHeight="1">
       <c r="A101" s="6"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
@@ -5470,7 +5468,7 @@
       <c r="P101" s="3"/>
       <c r="Q101" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
+    <row r="102" spans="1:17" ht="18.75" customHeight="1">
       <c r="A102" s="6"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
@@ -5489,7 +5487,7 @@
       <c r="P102" s="3"/>
       <c r="Q102" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
+    <row r="103" spans="1:17" ht="18.75" customHeight="1">
       <c r="A103" s="6"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
@@ -5508,7 +5506,7 @@
       <c r="P103" s="3"/>
       <c r="Q103" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
+    <row r="104" spans="1:17" ht="18.75" customHeight="1">
       <c r="A104" s="6"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
@@ -5527,7 +5525,7 @@
       <c r="P104" s="3"/>
       <c r="Q104" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
+    <row r="105" spans="1:17" ht="18.75" customHeight="1">
       <c r="A105" s="6"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
@@ -5546,7 +5544,7 @@
       <c r="P105" s="3"/>
       <c r="Q105" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75">
+    <row r="106" spans="1:17" ht="18.75" customHeight="1">
       <c r="A106" s="6"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
@@ -5565,7 +5563,7 @@
       <c r="P106" s="3"/>
       <c r="Q106" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75">
+    <row r="107" spans="1:17" ht="18.75" customHeight="1">
       <c r="A107" s="6"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
@@ -5584,7 +5582,7 @@
       <c r="P107" s="3"/>
       <c r="Q107" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75">
+    <row r="108" spans="1:17" ht="18.75" customHeight="1">
       <c r="A108" s="6"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
@@ -5603,7 +5601,7 @@
       <c r="P108" s="3"/>
       <c r="Q108" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75">
+    <row r="109" spans="1:17" ht="18.75" customHeight="1">
       <c r="A109" s="6"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
@@ -5622,7 +5620,7 @@
       <c r="P109" s="3"/>
       <c r="Q109" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75">
+    <row r="110" spans="1:17" ht="18.75" customHeight="1">
       <c r="A110" s="6"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
@@ -5641,7 +5639,7 @@
       <c r="P110" s="3"/>
       <c r="Q110" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75">
+    <row r="111" spans="1:17" ht="18.75" customHeight="1">
       <c r="A111" s="6"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
@@ -5660,7 +5658,7 @@
       <c r="P111" s="3"/>
       <c r="Q111" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75">
+    <row r="112" spans="1:17" ht="18.75" customHeight="1">
       <c r="A112" s="6"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
@@ -5679,7 +5677,7 @@
       <c r="P112" s="3"/>
       <c r="Q112" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18.75">
+    <row r="113" spans="1:17" ht="18.75" customHeight="1">
       <c r="A113" s="6"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
@@ -5698,7 +5696,7 @@
       <c r="P113" s="3"/>
       <c r="Q113" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75">
+    <row r="114" spans="1:17" ht="18.75" customHeight="1">
       <c r="A114" s="6"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
@@ -5717,7 +5715,7 @@
       <c r="P114" s="3"/>
       <c r="Q114" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18.75">
+    <row r="115" spans="1:17" ht="18.75" customHeight="1">
       <c r="A115" s="6"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
@@ -5736,7 +5734,7 @@
       <c r="P115" s="3"/>
       <c r="Q115" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18.75">
+    <row r="116" spans="1:17" ht="18.75" customHeight="1">
       <c r="A116" s="6"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
@@ -5755,7 +5753,7 @@
       <c r="P116" s="3"/>
       <c r="Q116" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18.75">
+    <row r="117" spans="1:17" ht="18.75" customHeight="1">
       <c r="A117" s="6"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
@@ -5774,7 +5772,7 @@
       <c r="P117" s="3"/>
       <c r="Q117" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18.75">
+    <row r="118" spans="1:17" ht="18.75" customHeight="1">
       <c r="A118" s="6"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
@@ -5793,7 +5791,7 @@
       <c r="P118" s="3"/>
       <c r="Q118" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18.75">
+    <row r="119" spans="1:17" ht="18.75" customHeight="1">
       <c r="A119" s="6"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
@@ -5812,7 +5810,7 @@
       <c r="P119" s="3"/>
       <c r="Q119" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18.75">
+    <row r="120" spans="1:17" ht="18.75" customHeight="1">
       <c r="A120" s="6"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
@@ -5831,7 +5829,7 @@
       <c r="P120" s="3"/>
       <c r="Q120" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18.75">
+    <row r="121" spans="1:17" ht="18.75" customHeight="1">
       <c r="A121" s="6"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
@@ -5850,7 +5848,7 @@
       <c r="P121" s="3"/>
       <c r="Q121" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18.75">
+    <row r="122" spans="1:17" ht="18.75" customHeight="1">
       <c r="A122" s="6"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
@@ -5869,7 +5867,7 @@
       <c r="P122" s="3"/>
       <c r="Q122" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18.75">
+    <row r="123" spans="1:17" ht="18.75" customHeight="1">
       <c r="A123" s="6"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
@@ -5888,7 +5886,7 @@
       <c r="P123" s="3"/>
       <c r="Q123" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18.75">
+    <row r="124" spans="1:17" ht="18.75" customHeight="1">
       <c r="A124" s="6"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
@@ -5907,7 +5905,7 @@
       <c r="P124" s="3"/>
       <c r="Q124" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18.75">
+    <row r="125" spans="1:17" ht="18.75" customHeight="1">
       <c r="A125" s="6"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
@@ -5926,7 +5924,7 @@
       <c r="P125" s="3"/>
       <c r="Q125" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18.75">
+    <row r="126" spans="1:17" ht="18.75" customHeight="1">
       <c r="A126" s="6"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
@@ -5945,7 +5943,7 @@
       <c r="P126" s="3"/>
       <c r="Q126" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75">
+    <row r="127" spans="1:17" ht="18.75" customHeight="1">
       <c r="A127" s="6"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
@@ -5964,7 +5962,7 @@
       <c r="P127" s="3"/>
       <c r="Q127" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18.75">
+    <row r="128" spans="1:17" ht="18.75" customHeight="1">
       <c r="A128" s="6"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
@@ -5983,7 +5981,7 @@
       <c r="P128" s="3"/>
       <c r="Q128" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18.75">
+    <row r="129" spans="1:17" ht="18.75" customHeight="1">
       <c r="A129" s="6"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
@@ -6002,7 +6000,7 @@
       <c r="P129" s="3"/>
       <c r="Q129" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18.75">
+    <row r="130" spans="1:17" ht="18.75" customHeight="1">
       <c r="A130" s="6"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
@@ -6021,7 +6019,7 @@
       <c r="P130" s="3"/>
       <c r="Q130" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18.75">
+    <row r="131" spans="1:17" ht="18.75" customHeight="1">
       <c r="A131" s="6"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
@@ -6040,7 +6038,7 @@
       <c r="P131" s="3"/>
       <c r="Q131" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="18.75">
+    <row r="132" spans="1:17" ht="18.75" customHeight="1">
       <c r="A132" s="6"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
@@ -6059,7 +6057,7 @@
       <c r="P132" s="3"/>
       <c r="Q132" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="18.75">
+    <row r="133" spans="1:17" ht="18.75" customHeight="1">
       <c r="A133" s="6"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
@@ -6078,7 +6076,7 @@
       <c r="P133" s="3"/>
       <c r="Q133" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="18.75">
+    <row r="134" spans="1:17" ht="18.75" customHeight="1">
       <c r="A134" s="6"/>
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
@@ -6097,7 +6095,7 @@
       <c r="P134" s="3"/>
       <c r="Q134" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="18.75">
+    <row r="135" spans="1:17" ht="18.75" customHeight="1">
       <c r="A135" s="6"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
@@ -6116,7 +6114,7 @@
       <c r="P135" s="3"/>
       <c r="Q135" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18.75">
+    <row r="136" spans="1:17" ht="18.75" customHeight="1">
       <c r="A136" s="6"/>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
@@ -6135,7 +6133,7 @@
       <c r="P136" s="3"/>
       <c r="Q136" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="18.75">
+    <row r="137" spans="1:17" ht="18.75" customHeight="1">
       <c r="A137" s="6"/>
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
@@ -6154,7 +6152,7 @@
       <c r="P137" s="3"/>
       <c r="Q137" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="18.75">
+    <row r="138" spans="1:17" ht="18.75" customHeight="1">
       <c r="A138" s="6"/>
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
@@ -6173,7 +6171,7 @@
       <c r="P138" s="3"/>
       <c r="Q138" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="18.75">
+    <row r="139" spans="1:17" ht="18.75" customHeight="1">
       <c r="A139" s="6"/>
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
@@ -6192,7 +6190,7 @@
       <c r="P139" s="3"/>
       <c r="Q139" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="18.75">
+    <row r="140" spans="1:17" ht="18.75" customHeight="1">
       <c r="A140" s="6"/>
       <c r="B140" s="3"/>
       <c r="C140" s="3"/>
@@ -6211,7 +6209,7 @@
       <c r="P140" s="3"/>
       <c r="Q140" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="18.75">
+    <row r="141" spans="1:17" ht="18.75" customHeight="1">
       <c r="A141" s="6"/>
       <c r="B141" s="3"/>
       <c r="C141" s="3"/>
@@ -6230,7 +6228,7 @@
       <c r="P141" s="3"/>
       <c r="Q141" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="18.75">
+    <row r="142" spans="1:17" ht="18.75" customHeight="1">
       <c r="A142" s="6"/>
       <c r="B142" s="3"/>
       <c r="C142" s="3"/>
@@ -6249,7 +6247,7 @@
       <c r="P142" s="3"/>
       <c r="Q142" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="18.75">
+    <row r="143" spans="1:17" ht="18.75" customHeight="1">
       <c r="A143" s="6"/>
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
@@ -6268,7 +6266,7 @@
       <c r="P143" s="3"/>
       <c r="Q143" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="18.75">
+    <row r="144" spans="1:17" ht="18.75" customHeight="1">
       <c r="A144" s="6"/>
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
@@ -6287,7 +6285,7 @@
       <c r="P144" s="3"/>
       <c r="Q144" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="18.75">
+    <row r="145" spans="1:17" ht="18.75" customHeight="1">
       <c r="A145" s="6"/>
       <c r="B145" s="3"/>
       <c r="C145" s="3"/>
@@ -6306,7 +6304,7 @@
       <c r="P145" s="3"/>
       <c r="Q145" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="18.75">
+    <row r="146" spans="1:17" ht="18.75" customHeight="1">
       <c r="A146" s="6"/>
       <c r="B146" s="3"/>
       <c r="C146" s="3"/>
@@ -6325,7 +6323,7 @@
       <c r="P146" s="3"/>
       <c r="Q146" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="18.75">
+    <row r="147" spans="1:17" ht="18.75" customHeight="1">
       <c r="A147" s="6"/>
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
@@ -6344,7 +6342,7 @@
       <c r="P147" s="3"/>
       <c r="Q147" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="18.75">
+    <row r="148" spans="1:17" ht="18.75" customHeight="1">
       <c r="A148" s="6"/>
       <c r="B148" s="3"/>
       <c r="C148" s="3"/>
@@ -6363,7 +6361,7 @@
       <c r="P148" s="3"/>
       <c r="Q148" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="18.75">
+    <row r="149" spans="1:17" ht="18.75" customHeight="1">
       <c r="A149" s="6"/>
       <c r="B149" s="3"/>
       <c r="C149" s="3"/>
@@ -6382,7 +6380,7 @@
       <c r="P149" s="3"/>
       <c r="Q149" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="18.75">
+    <row r="150" spans="1:17" ht="18.75" customHeight="1">
       <c r="A150" s="6"/>
       <c r="B150" s="3"/>
       <c r="C150" s="3"/>
@@ -6401,7 +6399,7 @@
       <c r="P150" s="3"/>
       <c r="Q150" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="18.75">
+    <row r="151" spans="1:17" ht="18.75" customHeight="1">
       <c r="A151" s="6"/>
       <c r="B151" s="3"/>
       <c r="C151" s="3"/>

</xml_diff>

<commit_message>
sergio arroyo agregó su regional
</commit_message>
<xml_diff>
--- a/Nomina.xlsx
+++ b/Nomina.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20390"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max-Soria\Desktop\udabol\Proyecto\UDABOL_202202\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\UDABOL\UDABOL_202202\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FFBE16-73BA-4302-98B4-09F357667607}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0F1FD9-6632-4EBF-BD28-FAE9B90EE9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="431">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -1748,12 +1748,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="13.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1">
@@ -2405,23 +2405,23 @@
   <dimension ref="A1:Q151"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="13" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="43.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="37.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="27.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="17" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="27.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="13.5546875" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" customHeight="1">
@@ -2544,7 +2544,9 @@
       <c r="K3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="5"/>
+      <c r="L3" s="5" t="s">
+        <v>430</v>
+      </c>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>

</xml_diff>

<commit_message>
Modificado por Kenneth Tercero - SCZ
</commit_message>
<xml_diff>
--- a/Nomina.xlsx
+++ b/Nomina.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3ba539708c964344/Desktop/Bryan/UDABOL_202202/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a-ktercero\Desktop\Desktop\Kenneth Tercero\UDABOL_202202\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{30AD40C0-E196-4A96-A29E-D4177A5662AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C68A7E03-DAEE-4BC2-A538-4674F5DD226B}"/>
   <bookViews>
-    <workbookView xWindow="924" yWindow="0" windowWidth="22116" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="22110" windowHeight="12360" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="432">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -1322,7 +1321,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -1743,7 +1742,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1753,12 +1752,12 @@
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1">
@@ -2385,7 +2384,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.6">
+    <row r="34" spans="1:6" ht="15.75">
       <c r="A34" s="12">
         <v>34</v>
       </c>
@@ -2408,30 +2407,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:Q151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="H16" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="37.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="17" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" customHeight="1">
@@ -3704,7 +3703,9 @@
       <c r="K31" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="L31" s="5"/>
+      <c r="L31" s="5" t="s">
+        <v>291</v>
+      </c>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>

</xml_diff>

<commit_message>
regional de sergio arroyo
</commit_message>
<xml_diff>
--- a/Nomina.xlsx
+++ b/Nomina.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20390"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max-Soria\Desktop\udabol\Proyecto\UDABOL_202202\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\UDABOL\UDABOL_202202\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F60F032-484C-4431-9369-33359B5673D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0278F791-2AA3-44C7-AAF0-6C3D28CFB32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="432">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -1753,12 +1753,12 @@
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1">
@@ -2385,7 +2385,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.75">
+    <row r="34" spans="1:6" ht="15.6">
       <c r="A34" s="12">
         <v>34</v>
       </c>
@@ -2415,23 +2415,23 @@
   <dimension ref="A1:Q151"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="13" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="43.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="17" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" customHeight="1">
@@ -2554,7 +2554,9 @@
       <c r="K3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="5"/>
+      <c r="L3" s="5" t="s">
+        <v>431</v>
+      </c>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>

</xml_diff>

<commit_message>
ME AGREGUE A LA NOMINA
</commit_message>
<xml_diff>
--- a/Nomina.xlsx
+++ b/Nomina.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MIKAELA NOELIA\Desktop\Udabol1\UDABOL_202202\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GIO\Desktop\UDABOL\UDABOL_202202\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F259B0FE-E0AA-46A2-A953-9E460ED8872A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513A5988-C3CA-49B5-BDBC-A7AD52502F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="435">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -1414,7 +1414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1447,9 +1447,6 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2398,7 +2395,7 @@
       <c r="A34" s="12">
         <v>34</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="10" t="s">
         <v>430</v>
       </c>
       <c r="C34" t="s">
@@ -2424,7 +2421,7 @@
   <dimension ref="A1:Q151"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2946,7 +2943,9 @@
       <c r="K12" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="L12" s="5"/>
+      <c r="L12" s="5" t="s">
+        <v>291</v>
+      </c>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>

</xml_diff>

<commit_message>
adicion de regional flor gutierrez
</commit_message>
<xml_diff>
--- a/Nomina.xlsx
+++ b/Nomina.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dictex\Desktop\udabol\UDABOL_202202\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\flor\A +\git\UDABOL_202202\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C4A62F-2E76-47A0-83C2-C42290C44909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1065" yWindow="-105" windowWidth="22080" windowHeight="13170" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="384" yWindow="0" windowWidth="12624" windowHeight="12360" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="437">
   <si>
     <t>Leonardo</t>
   </si>
@@ -1341,7 +1342,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy\ hh:mm"/>
   </numFmts>
@@ -1765,19 +1766,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1">
@@ -2404,7 +2405,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.75">
+    <row r="34" spans="1:6" ht="15.6">
       <c r="A34" s="1">
         <v>34</v>
       </c>
@@ -2424,7 +2425,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.75">
+    <row r="35" spans="1:6" ht="15.6">
       <c r="A35">
         <v>35</v>
       </c>
@@ -2448,27 +2449,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="13" style="6" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="30.140625" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" customWidth="1"/>
-    <col min="8" max="8" width="37.85546875" customWidth="1"/>
-    <col min="9" max="9" width="43.28515625" customWidth="1"/>
-    <col min="10" max="10" width="37.140625" customWidth="1"/>
-    <col min="11" max="12" width="27.28515625" customWidth="1"/>
-    <col min="13" max="17" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" customWidth="1"/>
+    <col min="6" max="6" width="30.109375" customWidth="1"/>
+    <col min="7" max="7" width="22.88671875" customWidth="1"/>
+    <col min="8" max="8" width="37.88671875" customWidth="1"/>
+    <col min="9" max="9" width="43.33203125" customWidth="1"/>
+    <col min="10" max="10" width="37.109375" customWidth="1"/>
+    <col min="11" max="12" width="27.33203125" customWidth="1"/>
+    <col min="13" max="17" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" customHeight="1">
@@ -3478,7 +3479,9 @@
       <c r="K24" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="L24" s="11"/>
+      <c r="L24" s="11" t="s">
+        <v>129</v>
+      </c>
       <c r="M24" s="9"/>
       <c r="N24" s="9"/>
       <c r="O24" s="9"/>

</xml_diff>

<commit_message>
Agregando sede en el Excel
</commit_message>
<xml_diff>
--- a/Nomina.xlsx
+++ b/Nomina.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows 10\Desktop\uda\UDABOL_202202\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mariella}\OneDrive\Desktop\Bryan\UDABOL_202202\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DBE335-D91B-4077-BEB7-9507B2269226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="924" yWindow="0" windowWidth="22116" windowHeight="12360" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="439">
   <si>
     <t>Leonardo</t>
   </si>
@@ -1339,12 +1340,15 @@
   </si>
   <si>
     <t xml:space="preserve">La Paz </t>
+  </si>
+  <si>
+    <t>ORURO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy\ hh:mm"/>
   </numFmts>
@@ -1765,19 +1769,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1">
@@ -2404,7 +2408,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.75">
+    <row r="34" spans="1:6" ht="15.6">
       <c r="A34" s="1">
         <v>34</v>
       </c>
@@ -2424,7 +2428,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.75">
+    <row r="35" spans="1:6" ht="15.6">
       <c r="A35">
         <v>35</v>
       </c>
@@ -2448,27 +2452,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="13" style="5" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="30.140625" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" customWidth="1"/>
-    <col min="8" max="8" width="37.85546875" customWidth="1"/>
-    <col min="9" max="9" width="43.28515625" customWidth="1"/>
-    <col min="10" max="10" width="37.140625" customWidth="1"/>
-    <col min="11" max="12" width="27.28515625" customWidth="1"/>
-    <col min="13" max="17" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" customWidth="1"/>
+    <col min="6" max="6" width="30.109375" customWidth="1"/>
+    <col min="7" max="7" width="22.88671875" customWidth="1"/>
+    <col min="8" max="8" width="37.88671875" customWidth="1"/>
+    <col min="9" max="9" width="43.33203125" customWidth="1"/>
+    <col min="10" max="10" width="37.109375" customWidth="1"/>
+    <col min="11" max="12" width="27.33203125" customWidth="1"/>
+    <col min="13" max="17" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" customHeight="1">
@@ -2720,7 +2724,9 @@
       <c r="K6" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="L6" s="10"/>
+      <c r="L6" s="10" t="s">
+        <v>438</v>
+      </c>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>

</xml_diff>

<commit_message>
Modificacion de Kenneth Tercero - SCZ
</commit_message>
<xml_diff>
--- a/Nomina.xlsx
+++ b/Nomina.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\windows 10\Desktop\Udabolsam\UDABOL_202202\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\UDABOL_202202\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244B2481-D979-46C0-B60F-97780C3722FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2470B5-4229-476D-93CA-9FC0DAF96C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="439">
   <si>
     <t>Leonardo</t>
   </si>
@@ -2466,13 +2466,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView tabSelected="1" topLeftCell="F19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13" style="5" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" customWidth="1"/>
@@ -2482,7 +2482,8 @@
     <col min="8" max="8" width="37.85546875" customWidth="1"/>
     <col min="9" max="9" width="43.28515625" customWidth="1"/>
     <col min="10" max="10" width="37.140625" customWidth="1"/>
-    <col min="11" max="12" width="27.28515625" customWidth="1"/>
+    <col min="11" max="11" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.28515625" customWidth="1"/>
     <col min="13" max="17" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3798,7 +3799,9 @@
       <c r="K31" s="10" t="s">
         <v>308</v>
       </c>
-      <c r="L31" s="10"/>
+      <c r="L31" s="10" t="s">
+        <v>197</v>
+      </c>
       <c r="M31" s="8"/>
       <c r="N31" s="8"/>
       <c r="O31" s="8"/>

</xml_diff>

<commit_message>
Adicion de Regionalidad Diego Dorado
</commit_message>
<xml_diff>
--- a/Nomina.xlsx
+++ b/Nomina.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KATY\Desktop\UDABOL ACTUALIZACION\UDABOL_202202\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97891759-B910-4286-8C72-9162FB34C78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="439">
   <si>
     <t>Leonardo</t>
   </si>
@@ -1348,7 +1342,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy\ hh:mm"/>
   </numFmts>
@@ -1773,14 +1767,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2463,11 +2457,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" topLeftCell="H33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L49" sqref="L49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -4545,7 +4539,9 @@
       <c r="K49" s="10" t="s">
         <v>422</v>
       </c>
-      <c r="L49" s="10"/>
+      <c r="L49" s="10" t="s">
+        <v>129</v>
+      </c>
       <c r="M49" s="8"/>
       <c r="N49" s="8"/>
       <c r="O49" s="8"/>

</xml_diff>

<commit_message>
La paz Diego cornejo
</commit_message>
<xml_diff>
--- a/Nomina.xlsx
+++ b/Nomina.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\UDABOL_202202\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC27215-52E4-43DC-ADD3-1867B3208953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11760" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="445">
   <si>
     <t>Leonardo</t>
   </si>
@@ -1358,12 +1352,15 @@
   </si>
   <si>
     <t>rsaucedo-es1@udabol.edu.bo</t>
+  </si>
+  <si>
+    <t>La paz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy\ hh:mm"/>
   </numFmts>
@@ -1836,26 +1833,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6328125" customWidth="1"/>
-    <col min="3" max="5" width="13.54296875" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1">
@@ -2482,7 +2479,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.5">
+    <row r="34" spans="1:6" ht="15.75">
       <c r="A34" s="1">
         <v>34</v>
       </c>
@@ -2502,7 +2499,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.5">
+    <row r="35" spans="1:6" ht="15.75">
       <c r="A35">
         <v>35</v>
       </c>
@@ -2526,28 +2523,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" topLeftCell="I28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="9.90625" customWidth="1"/>
-    <col min="4" max="4" width="9.36328125" customWidth="1"/>
-    <col min="5" max="5" width="15.90625" customWidth="1"/>
-    <col min="6" max="6" width="30.08984375" customWidth="1"/>
-    <col min="7" max="7" width="22.90625" customWidth="1"/>
-    <col min="8" max="8" width="37.90625" customWidth="1"/>
-    <col min="9" max="9" width="43.36328125" customWidth="1"/>
-    <col min="10" max="10" width="37.08984375" customWidth="1"/>
-    <col min="11" max="11" width="28.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.36328125" customWidth="1"/>
-    <col min="13" max="17" width="13.54296875" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="30.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" customWidth="1"/>
+    <col min="8" max="8" width="37.85546875" customWidth="1"/>
+    <col min="9" max="9" width="43.42578125" customWidth="1"/>
+    <col min="10" max="10" width="37.140625" customWidth="1"/>
+    <col min="11" max="11" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.42578125" customWidth="1"/>
+    <col min="13" max="17" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" customHeight="1">
@@ -4116,7 +4113,9 @@
       <c r="K37" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="L37" s="10"/>
+      <c r="L37" s="10" t="s">
+        <v>444</v>
+      </c>
       <c r="M37" s="8"/>
       <c r="N37" s="8"/>
       <c r="O37" s="8"/>
@@ -6627,8 +6626,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B52" r:id="rId1" xr:uid="{5CCA29A1-4312-40DB-97BF-352737FC896B}"/>
-    <hyperlink ref="K22" r:id="rId2" xr:uid="{7A4ED392-A942-426F-BDF6-8C6A8325C11D}"/>
+    <hyperlink ref="B52" r:id="rId1"/>
+    <hyperlink ref="K22" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>

</xml_diff>

<commit_message>
La Paz - Deymar
</commit_message>
<xml_diff>
--- a/Nomina.xlsx
+++ b/Nomina.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\UDABOL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DEYMAR HUARACHI\GABRIELU\UDABOL_202202\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E0B956-3DA5-4F5F-A2A9-413C42750E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="445">
   <si>
     <t>Leonardo</t>
   </si>
@@ -1365,7 +1366,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy\ hh:mm"/>
   </numFmts>
@@ -1845,19 +1846,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1"/>
+    <col min="3" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1">
@@ -2484,7 +2485,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.75">
+    <row r="34" spans="1:6" ht="15.6">
       <c r="A34" s="1">
         <v>34</v>
       </c>
@@ -2504,7 +2505,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.75">
+    <row r="35" spans="1:6" ht="15.6">
       <c r="A35">
         <v>35</v>
       </c>
@@ -2528,28 +2529,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q151"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="30.140625" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" customWidth="1"/>
-    <col min="8" max="8" width="37.85546875" customWidth="1"/>
-    <col min="9" max="9" width="43.42578125" customWidth="1"/>
-    <col min="10" max="10" width="37.140625" customWidth="1"/>
-    <col min="11" max="11" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.42578125" customWidth="1"/>
-    <col min="13" max="17" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" customWidth="1"/>
+    <col min="6" max="6" width="30.109375" customWidth="1"/>
+    <col min="7" max="7" width="22.88671875" customWidth="1"/>
+    <col min="8" max="8" width="37.88671875" customWidth="1"/>
+    <col min="9" max="9" width="43.44140625" customWidth="1"/>
+    <col min="10" max="10" width="37.109375" customWidth="1"/>
+    <col min="11" max="11" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.44140625" customWidth="1"/>
+    <col min="13" max="17" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" customHeight="1">
@@ -4302,7 +4303,9 @@
       <c r="K41" s="10" t="s">
         <v>371</v>
       </c>
-      <c r="L41" s="10"/>
+      <c r="L41" s="10" t="s">
+        <v>129</v>
+      </c>
       <c r="M41" s="8"/>
       <c r="N41" s="8"/>
       <c r="O41" s="8"/>
@@ -6657,8 +6660,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B52" r:id="rId1"/>
-    <hyperlink ref="K22" r:id="rId2"/>
+    <hyperlink ref="B52" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="K22" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>

</xml_diff>

<commit_message>
ADicion de 3 alumno y poryecto final
</commit_message>
<xml_diff>
--- a/Nomina.xlsx
+++ b/Nomina.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rogerruizescobar/Documents/UDABOL/UDABOL_202202/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86988BDA-1407-174D-9F51-2C3BD07C37C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8638878C-ACAA-9445-B7FC-6EA603955EC9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="462">
   <si>
     <t>Leonardo</t>
   </si>
@@ -1372,12 +1372,6 @@
     <t>Plinio Alex Gonzalo Quipe</t>
   </si>
   <si>
-    <t>Usuario 55</t>
-  </si>
-  <si>
-    <t>Usuario 56</t>
-  </si>
-  <si>
     <t>Grupo</t>
   </si>
   <si>
@@ -1406,6 +1400,18 @@
   </si>
   <si>
     <t>Presentacion Operaciones con usuarios</t>
+  </si>
+  <si>
+    <t>STEFANIA CHOQUE APAZA</t>
+  </si>
+  <si>
+    <t>MARCO ANTONIO CANQUI OROSCO</t>
+  </si>
+  <si>
+    <t>ROLANDO LISARASO ARNEZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joel Uria </t>
   </si>
 </sst>
 </file>
@@ -1497,7 +1503,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1520,12 +1526,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1575,6 +1629,27 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -2575,8 +2650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q56" sqref="Q56"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P53" sqref="P53:P54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2636,7 +2711,7 @@
       </c>
       <c r="N1" s="7"/>
       <c r="O1" s="7" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
@@ -2690,7 +2765,7 @@
         <v>0</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="Q2" s="8"/>
       <c r="R2" s="8"/>
@@ -2742,7 +2817,9 @@
         <f>MOD(N3,10)</f>
         <v>0</v>
       </c>
-      <c r="P3" s="8"/>
+      <c r="P3" s="8" t="s">
+        <v>453</v>
+      </c>
       <c r="Q3" s="8"/>
       <c r="R3" s="8"/>
     </row>
@@ -2791,7 +2868,9 @@
         <f>MOD(N4,10)</f>
         <v>0</v>
       </c>
-      <c r="P4" s="8"/>
+      <c r="P4" s="8" t="s">
+        <v>453</v>
+      </c>
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
     </row>
@@ -2840,7 +2919,9 @@
         <f>MOD(N5,10)</f>
         <v>0</v>
       </c>
-      <c r="P5" s="8"/>
+      <c r="P5" s="8" t="s">
+        <v>453</v>
+      </c>
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
     </row>
@@ -2891,7 +2972,9 @@
         <f>MOD(N6,10)</f>
         <v>0</v>
       </c>
-      <c r="P6" s="8"/>
+      <c r="P6" s="8" t="s">
+        <v>453</v>
+      </c>
       <c r="Q6" s="8"/>
       <c r="R6" s="8"/>
     </row>
@@ -2942,7 +3025,9 @@
         <f>MOD(N7,10)</f>
         <v>1</v>
       </c>
-      <c r="P7" s="8"/>
+      <c r="P7" s="8" t="s">
+        <v>454</v>
+      </c>
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
     </row>
@@ -2994,7 +3079,7 @@
         <v>1</v>
       </c>
       <c r="P8" s="8" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="Q8" s="8"/>
       <c r="R8" s="8"/>
@@ -3046,7 +3131,9 @@
         <f>MOD(N9,10)</f>
         <v>1</v>
       </c>
-      <c r="P9" s="8"/>
+      <c r="P9" s="8" t="s">
+        <v>454</v>
+      </c>
       <c r="Q9" s="8"/>
       <c r="R9" s="8"/>
     </row>
@@ -3097,7 +3184,9 @@
         <f>MOD(N10,10)</f>
         <v>1</v>
       </c>
-      <c r="P10" s="8"/>
+      <c r="P10" s="8" t="s">
+        <v>454</v>
+      </c>
       <c r="Q10" s="8"/>
       <c r="R10" s="8"/>
     </row>
@@ -3148,7 +3237,9 @@
         <f>MOD(N11,10)</f>
         <v>1</v>
       </c>
-      <c r="P11" s="8"/>
+      <c r="P11" s="8" t="s">
+        <v>454</v>
+      </c>
       <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
     </row>
@@ -3199,7 +3290,9 @@
         <f>MOD(N12,10)</f>
         <v>1</v>
       </c>
-      <c r="P12" s="8"/>
+      <c r="P12" s="8" t="s">
+        <v>454</v>
+      </c>
       <c r="Q12" s="8"/>
       <c r="R12" s="8"/>
     </row>
@@ -3251,7 +3344,7 @@
         <v>2</v>
       </c>
       <c r="P13" s="8" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="Q13" s="8"/>
       <c r="R13" s="8"/>
@@ -3301,7 +3394,9 @@
         <f>MOD(N14,10)</f>
         <v>2</v>
       </c>
-      <c r="P14" s="8"/>
+      <c r="P14" s="8" t="s">
+        <v>449</v>
+      </c>
       <c r="Q14" s="8"/>
       <c r="R14" s="8"/>
     </row>
@@ -3352,7 +3447,9 @@
         <f>MOD(N15,10)</f>
         <v>2</v>
       </c>
-      <c r="P15" s="8"/>
+      <c r="P15" s="8" t="s">
+        <v>449</v>
+      </c>
       <c r="Q15" s="8"/>
       <c r="R15" s="8"/>
     </row>
@@ -3403,7 +3500,9 @@
         <f>MOD(N16,10)</f>
         <v>2</v>
       </c>
-      <c r="P16" s="8"/>
+      <c r="P16" s="8" t="s">
+        <v>449</v>
+      </c>
       <c r="Q16" s="8"/>
       <c r="R16" s="8"/>
     </row>
@@ -3454,7 +3553,9 @@
         <f>MOD(N17,10)</f>
         <v>2</v>
       </c>
-      <c r="P17" s="8"/>
+      <c r="P17" s="8" t="s">
+        <v>449</v>
+      </c>
       <c r="Q17" s="8"/>
       <c r="R17" s="8"/>
     </row>
@@ -3483,7 +3584,9 @@
         <f>MOD(N18,10)</f>
         <v>2</v>
       </c>
-      <c r="P18" s="8"/>
+      <c r="P18" s="8" t="s">
+        <v>449</v>
+      </c>
       <c r="Q18" s="8"/>
       <c r="R18" s="8"/>
     </row>
@@ -3535,7 +3638,7 @@
         <v>3</v>
       </c>
       <c r="P19" s="8" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="Q19" s="8"/>
       <c r="R19" s="8"/>
@@ -3587,7 +3690,9 @@
         <f>MOD(N20,10)</f>
         <v>3</v>
       </c>
-      <c r="P20" s="8"/>
+      <c r="P20" s="8" t="s">
+        <v>450</v>
+      </c>
       <c r="Q20" s="8"/>
       <c r="R20" s="8"/>
     </row>
@@ -3638,7 +3743,9 @@
         <f>MOD(N21,10)</f>
         <v>3</v>
       </c>
-      <c r="P21" s="8"/>
+      <c r="P21" s="8" t="s">
+        <v>450</v>
+      </c>
       <c r="Q21" s="8"/>
       <c r="R21" s="8"/>
     </row>
@@ -3689,7 +3796,9 @@
         <f>MOD(N22,10)</f>
         <v>3</v>
       </c>
-      <c r="P22" s="8"/>
+      <c r="P22" s="8" t="s">
+        <v>450</v>
+      </c>
       <c r="Q22" s="8"/>
       <c r="R22" s="8"/>
     </row>
@@ -3740,7 +3849,9 @@
         <f>MOD(N23,10)</f>
         <v>3</v>
       </c>
-      <c r="P23" s="8"/>
+      <c r="P23" s="8" t="s">
+        <v>450</v>
+      </c>
       <c r="Q23" s="8"/>
       <c r="R23" s="8"/>
     </row>
@@ -3769,7 +3880,9 @@
         <f>MOD(N24,10)</f>
         <v>3</v>
       </c>
-      <c r="P24" s="8"/>
+      <c r="P24" s="8" t="s">
+        <v>450</v>
+      </c>
       <c r="Q24" s="8"/>
       <c r="R24" s="8"/>
     </row>
@@ -3821,7 +3934,7 @@
         <v>4</v>
       </c>
       <c r="P25" s="8" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="Q25" s="8"/>
       <c r="R25" s="8"/>
@@ -3873,7 +3986,9 @@
         <f>MOD(N26,10)</f>
         <v>4</v>
       </c>
-      <c r="P26" s="8"/>
+      <c r="P26" s="8" t="s">
+        <v>451</v>
+      </c>
       <c r="Q26" s="8"/>
       <c r="R26" s="8"/>
     </row>
@@ -3924,7 +4039,9 @@
         <f>MOD(N27,10)</f>
         <v>4</v>
       </c>
-      <c r="P27" s="8"/>
+      <c r="P27" s="8" t="s">
+        <v>451</v>
+      </c>
       <c r="Q27" s="8"/>
       <c r="R27" s="8"/>
     </row>
@@ -3975,7 +4092,9 @@
         <f>MOD(N28,10)</f>
         <v>4</v>
       </c>
-      <c r="P28" s="8"/>
+      <c r="P28" s="8" t="s">
+        <v>451</v>
+      </c>
       <c r="Q28" s="8"/>
       <c r="R28" s="8"/>
     </row>
@@ -4026,7 +4145,9 @@
         <f>MOD(N29,10)</f>
         <v>4</v>
       </c>
-      <c r="P29" s="8"/>
+      <c r="P29" s="8" t="s">
+        <v>451</v>
+      </c>
       <c r="Q29" s="8"/>
       <c r="R29" s="8"/>
     </row>
@@ -4055,7 +4176,9 @@
         <f>MOD(N30,10)</f>
         <v>4</v>
       </c>
-      <c r="P30" s="8"/>
+      <c r="P30" s="8" t="s">
+        <v>451</v>
+      </c>
       <c r="Q30" s="8"/>
       <c r="R30" s="8"/>
     </row>
@@ -4107,7 +4230,7 @@
         <v>5</v>
       </c>
       <c r="P31" s="8" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="Q31" s="8"/>
       <c r="R31" s="8"/>
@@ -4159,7 +4282,9 @@
         <f>MOD(N32,10)</f>
         <v>5</v>
       </c>
-      <c r="P32" s="8"/>
+      <c r="P32" s="8" t="s">
+        <v>452</v>
+      </c>
       <c r="Q32" s="8"/>
       <c r="R32" s="8"/>
     </row>
@@ -4210,7 +4335,9 @@
         <f>MOD(N33,10)</f>
         <v>5</v>
       </c>
-      <c r="P33" s="8"/>
+      <c r="P33" s="8" t="s">
+        <v>452</v>
+      </c>
       <c r="Q33" s="8"/>
       <c r="R33" s="8"/>
     </row>
@@ -4261,7 +4388,9 @@
         <f>MOD(N34,10)</f>
         <v>5</v>
       </c>
-      <c r="P34" s="8"/>
+      <c r="P34" s="8" t="s">
+        <v>452</v>
+      </c>
       <c r="Q34" s="8"/>
       <c r="R34" s="8"/>
     </row>
@@ -4312,7 +4441,9 @@
         <f>MOD(N35,10)</f>
         <v>5</v>
       </c>
-      <c r="P35" s="8"/>
+      <c r="P35" s="8" t="s">
+        <v>452</v>
+      </c>
       <c r="Q35" s="8"/>
       <c r="R35" s="8"/>
     </row>
@@ -4321,7 +4452,7 @@
         <v>55</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>448</v>
+        <v>458</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
@@ -4341,7 +4472,9 @@
         <f>MOD(N36,10)</f>
         <v>5</v>
       </c>
-      <c r="P36" s="8"/>
+      <c r="P36" s="8" t="s">
+        <v>452</v>
+      </c>
       <c r="Q36" s="8"/>
       <c r="R36" s="8"/>
     </row>
@@ -4393,7 +4526,7 @@
         <v>6</v>
       </c>
       <c r="P37" s="8" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="Q37" s="8"/>
       <c r="R37" s="8"/>
@@ -4445,7 +4578,9 @@
         <f>MOD(N38,10)</f>
         <v>6</v>
       </c>
-      <c r="P38" s="8"/>
+      <c r="P38" s="8" t="s">
+        <v>455</v>
+      </c>
       <c r="Q38" s="8"/>
       <c r="R38" s="8"/>
     </row>
@@ -4496,7 +4631,9 @@
         <f>MOD(N39,10)</f>
         <v>6</v>
       </c>
-      <c r="P39" s="8"/>
+      <c r="P39" s="8" t="s">
+        <v>455</v>
+      </c>
       <c r="Q39" s="8"/>
       <c r="R39" s="8"/>
     </row>
@@ -4547,7 +4684,9 @@
         <f>MOD(N40,10)</f>
         <v>6</v>
       </c>
-      <c r="P40" s="8"/>
+      <c r="P40" s="8" t="s">
+        <v>455</v>
+      </c>
       <c r="Q40" s="8"/>
       <c r="R40" s="8"/>
     </row>
@@ -4596,7 +4735,9 @@
         <f>MOD(N41,10)</f>
         <v>6</v>
       </c>
-      <c r="P41" s="8"/>
+      <c r="P41" s="8" t="s">
+        <v>455</v>
+      </c>
       <c r="Q41" s="8"/>
       <c r="R41" s="8"/>
     </row>
@@ -4605,7 +4746,7 @@
         <v>56</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>449</v>
+        <v>459</v>
       </c>
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
@@ -4625,7 +4766,9 @@
         <f>MOD(N42,10)</f>
         <v>6</v>
       </c>
-      <c r="P42" s="8"/>
+      <c r="P42" s="8" t="s">
+        <v>455</v>
+      </c>
       <c r="Q42" s="8"/>
       <c r="R42" s="8"/>
     </row>
@@ -4677,7 +4820,7 @@
         <v>7</v>
       </c>
       <c r="P43" s="8" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="Q43" s="8"/>
       <c r="R43" s="8"/>
@@ -4729,7 +4872,9 @@
         <f>MOD(N44,10)</f>
         <v>7</v>
       </c>
-      <c r="P44" s="8"/>
+      <c r="P44" s="8" t="s">
+        <v>454</v>
+      </c>
       <c r="Q44" s="8"/>
       <c r="R44" s="8"/>
     </row>
@@ -4780,7 +4925,9 @@
         <f>MOD(N45,10)</f>
         <v>7</v>
       </c>
-      <c r="P45" s="8"/>
+      <c r="P45" s="8" t="s">
+        <v>454</v>
+      </c>
       <c r="Q45" s="8"/>
       <c r="R45" s="8"/>
     </row>
@@ -4831,7 +4978,9 @@
         <f>MOD(N46,10)</f>
         <v>7</v>
       </c>
-      <c r="P46" s="8"/>
+      <c r="P46" s="8" t="s">
+        <v>454</v>
+      </c>
       <c r="Q46" s="8"/>
       <c r="R46" s="8"/>
     </row>
@@ -4882,559 +5031,601 @@
         <f>MOD(N47,10)</f>
         <v>7</v>
       </c>
-      <c r="P47" s="8"/>
+      <c r="P47" s="8" t="s">
+        <v>454</v>
+      </c>
       <c r="Q47" s="8"/>
       <c r="R47" s="8"/>
     </row>
     <row r="48" spans="1:18" ht="18.75" customHeight="1">
-      <c r="A48" s="18">
-        <v>38</v>
-      </c>
-      <c r="B48" s="9">
-        <v>44817.345902777801</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>350</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>351</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>351</v>
-      </c>
-      <c r="F48" s="10" t="s">
-        <v>352</v>
-      </c>
-      <c r="G48" s="10" t="s">
-        <v>350</v>
-      </c>
-      <c r="H48" s="10" t="s">
-        <v>353</v>
-      </c>
-      <c r="I48" s="10" t="s">
-        <v>354</v>
-      </c>
-      <c r="J48" s="10" t="s">
-        <v>355</v>
-      </c>
-      <c r="K48" s="10" t="s">
-        <v>350</v>
-      </c>
-      <c r="L48" s="10" t="s">
-        <v>356</v>
-      </c>
-      <c r="M48" s="10" t="s">
-        <v>129</v>
-      </c>
+      <c r="A48" s="22">
+        <v>57</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>460</v>
+      </c>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="10"/>
+      <c r="K48" s="10"/>
+      <c r="L48" s="10"/>
+      <c r="M48" s="10"/>
       <c r="N48" s="10">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="O48" s="10">
         <f>MOD(N48,10)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P48" s="8" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="Q48" s="8"/>
       <c r="R48" s="8"/>
     </row>
     <row r="49" spans="1:18" ht="18.75" customHeight="1">
       <c r="A49" s="18">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B49" s="9">
-        <v>44819.794398148202</v>
+        <v>44817.345902777801</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>417</v>
+        <v>350</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>39</v>
+        <v>351</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>40</v>
+        <v>351</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>341</v>
+        <v>352</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>417</v>
+        <v>350</v>
       </c>
       <c r="H49" s="10" t="s">
-        <v>418</v>
+        <v>353</v>
       </c>
       <c r="I49" s="10" t="s">
-        <v>419</v>
+        <v>354</v>
       </c>
       <c r="J49" s="10" t="s">
-        <v>420</v>
+        <v>355</v>
       </c>
       <c r="K49" s="10" t="s">
-        <v>417</v>
+        <v>350</v>
       </c>
       <c r="L49" s="10" t="s">
-        <v>421</v>
+        <v>356</v>
       </c>
       <c r="M49" s="10" t="s">
         <v>129</v>
       </c>
       <c r="N49" s="10">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="O49" s="10">
         <f>MOD(N49,10)</f>
         <v>8</v>
       </c>
-      <c r="P49" s="8"/>
+      <c r="P49" s="8" t="s">
+        <v>456</v>
+      </c>
       <c r="Q49" s="8"/>
       <c r="R49" s="8"/>
     </row>
     <row r="50" spans="1:18" ht="18.75" customHeight="1">
       <c r="A50" s="18">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="B50" s="9">
-        <v>44816.900972222204</v>
+        <v>44819.794398148202</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>168</v>
+        <v>417</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>169</v>
+        <v>341</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>168</v>
+        <v>417</v>
       </c>
       <c r="H50" s="10" t="s">
-        <v>170</v>
+        <v>418</v>
       </c>
       <c r="I50" s="10" t="s">
-        <v>171</v>
+        <v>419</v>
       </c>
       <c r="J50" s="10" t="s">
-        <v>172</v>
+        <v>420</v>
       </c>
       <c r="K50" s="10" t="s">
-        <v>168</v>
+        <v>417</v>
       </c>
       <c r="L50" s="10" t="s">
-        <v>173</v>
+        <v>421</v>
       </c>
       <c r="M50" s="10" t="s">
-        <v>174</v>
+        <v>129</v>
       </c>
       <c r="N50" s="10">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="O50" s="10">
         <f>MOD(N50,10)</f>
         <v>8</v>
       </c>
-      <c r="P50" s="8"/>
+      <c r="P50" s="8" t="s">
+        <v>456</v>
+      </c>
       <c r="Q50" s="8"/>
       <c r="R50" s="8"/>
     </row>
     <row r="51" spans="1:18" ht="18.75" customHeight="1">
       <c r="A51" s="18">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B51" s="9">
-        <v>44816.903657407398</v>
+        <v>44816.900972222204</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>233</v>
+        <v>168</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>234</v>
+        <v>169</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>233</v>
+        <v>168</v>
       </c>
       <c r="H51" s="10" t="s">
-        <v>235</v>
+        <v>170</v>
       </c>
       <c r="I51" s="10" t="s">
-        <v>236</v>
+        <v>171</v>
       </c>
       <c r="J51" s="10" t="s">
-        <v>237</v>
+        <v>172</v>
       </c>
       <c r="K51" s="10" t="s">
-        <v>233</v>
+        <v>168</v>
       </c>
       <c r="L51" s="10" t="s">
-        <v>238</v>
+        <v>173</v>
       </c>
       <c r="M51" s="10" t="s">
-        <v>129</v>
+        <v>174</v>
       </c>
       <c r="N51" s="10">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="O51" s="10">
         <f>MOD(N51,10)</f>
         <v>8</v>
       </c>
-      <c r="P51" s="8"/>
+      <c r="P51" s="8" t="s">
+        <v>456</v>
+      </c>
       <c r="Q51" s="8"/>
       <c r="R51" s="8"/>
     </row>
     <row r="52" spans="1:18" ht="18.75" customHeight="1">
       <c r="A52" s="18">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B52" s="9">
-        <v>44816.906689814801</v>
+        <v>44816.903657407398</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>289</v>
+        <v>233</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>105</v>
+        <v>67</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>106</v>
+        <v>2</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>20</v>
+        <v>234</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>290</v>
+        <v>233</v>
       </c>
       <c r="H52" s="10" t="s">
-        <v>291</v>
+        <v>235</v>
       </c>
       <c r="I52" s="10" t="s">
-        <v>292</v>
+        <v>236</v>
       </c>
       <c r="J52" s="10" t="s">
-        <v>293</v>
+        <v>237</v>
       </c>
       <c r="K52" s="10" t="s">
-        <v>289</v>
+        <v>233</v>
       </c>
       <c r="L52" s="10" t="s">
-        <v>290</v>
+        <v>238</v>
       </c>
       <c r="M52" s="10" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="N52" s="10">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="O52" s="10">
         <f>MOD(N52,10)</f>
         <v>8</v>
       </c>
-      <c r="P52" s="8"/>
+      <c r="P52" s="8" t="s">
+        <v>456</v>
+      </c>
       <c r="Q52" s="8"/>
       <c r="R52" s="8"/>
     </row>
     <row r="53" spans="1:18" ht="18.75" customHeight="1">
       <c r="A53" s="18">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="B53" s="9">
-        <v>44819.812349537002</v>
+        <v>44816.906689814801</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>422</v>
+        <v>289</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>423</v>
+        <v>105</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>424</v>
+        <v>106</v>
       </c>
       <c r="F53" s="10" t="s">
-        <v>425</v>
+        <v>20</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>426</v>
+        <v>290</v>
       </c>
       <c r="H53" s="10" t="s">
-        <v>427</v>
+        <v>291</v>
       </c>
       <c r="I53" s="10" t="s">
-        <v>428</v>
+        <v>292</v>
       </c>
       <c r="J53" s="10" t="s">
-        <v>427</v>
+        <v>293</v>
       </c>
       <c r="K53" s="10" t="s">
-        <v>422</v>
+        <v>289</v>
       </c>
       <c r="L53" s="10" t="s">
-        <v>429</v>
+        <v>290</v>
       </c>
       <c r="M53" s="10" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="N53" s="10">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="O53" s="10">
         <f>MOD(N53,10)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P53" s="8" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="Q53" s="8"/>
       <c r="R53" s="8"/>
     </row>
     <row r="54" spans="1:18" ht="18.75" customHeight="1">
-      <c r="A54" s="18">
-        <v>19</v>
-      </c>
-      <c r="B54" s="9">
-        <v>44816.903692129599</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="E54" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="F54" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="G54" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="H54" s="10" t="s">
-        <v>241</v>
-      </c>
-      <c r="I54" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="J54" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="K54" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="L54" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="M54" s="10" t="s">
-        <v>129</v>
-      </c>
+      <c r="A54" s="22">
+        <v>58</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>461</v>
+      </c>
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="10"/>
+      <c r="H54" s="10"/>
+      <c r="I54" s="10"/>
+      <c r="J54" s="10"/>
+      <c r="K54" s="10"/>
+      <c r="L54" s="10"/>
+      <c r="M54" s="10"/>
       <c r="N54" s="10">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="O54" s="10">
         <f>MOD(N54,10)</f>
-        <v>9</v>
-      </c>
-      <c r="P54" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="P54" s="8" t="s">
+        <v>456</v>
+      </c>
       <c r="Q54" s="8"/>
       <c r="R54" s="8"/>
     </row>
     <row r="55" spans="1:18" ht="18.75" customHeight="1">
       <c r="A55" s="18">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B55" s="9">
-        <v>44817.728460648199</v>
+        <v>44819.812349537002</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>357</v>
+        <v>422</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>358</v>
+        <v>423</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>359</v>
+        <v>424</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>360</v>
+        <v>425</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>361</v>
+        <v>426</v>
       </c>
       <c r="H55" s="10" t="s">
-        <v>362</v>
+        <v>427</v>
       </c>
       <c r="I55" s="10" t="s">
-        <v>363</v>
+        <v>428</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>364</v>
+        <v>427</v>
       </c>
       <c r="K55" s="10" t="s">
-        <v>361</v>
+        <v>422</v>
       </c>
       <c r="L55" s="10" t="s">
-        <v>357</v>
+        <v>429</v>
       </c>
       <c r="M55" s="10" t="s">
-        <v>197</v>
+        <v>129</v>
       </c>
       <c r="N55" s="10">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="O55" s="10">
         <f>MOD(N55,10)</f>
         <v>9</v>
       </c>
-      <c r="P55" s="8"/>
+      <c r="P55" s="8" t="s">
+        <v>457</v>
+      </c>
       <c r="Q55" s="8"/>
       <c r="R55" s="8"/>
     </row>
     <row r="56" spans="1:18" ht="18.75" customHeight="1">
       <c r="A56" s="18">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B56" s="9">
-        <v>44816.901365740698</v>
+        <v>44816.903692129599</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>175</v>
+        <v>239</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>176</v>
+        <v>103</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>177</v>
+        <v>104</v>
       </c>
       <c r="F56" s="10" t="s">
-        <v>178</v>
+        <v>102</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>179</v>
+        <v>240</v>
       </c>
       <c r="H56" s="10" t="s">
-        <v>180</v>
+        <v>241</v>
       </c>
       <c r="I56" s="10" t="s">
-        <v>181</v>
+        <v>242</v>
       </c>
       <c r="J56" s="10" t="s">
-        <v>181</v>
+        <v>242</v>
       </c>
       <c r="K56" s="10" t="s">
-        <v>175</v>
+        <v>239</v>
       </c>
       <c r="L56" s="10" t="s">
-        <v>179</v>
+        <v>240</v>
       </c>
       <c r="M56" s="10" t="s">
         <v>129</v>
       </c>
       <c r="N56" s="10">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="O56" s="10">
         <f>MOD(N56,10)</f>
         <v>9</v>
       </c>
-      <c r="P56" s="8"/>
+      <c r="P56" s="8" t="s">
+        <v>457</v>
+      </c>
       <c r="Q56" s="8"/>
       <c r="R56" s="8"/>
     </row>
     <row r="57" spans="1:18" ht="18.75" customHeight="1">
-      <c r="A57" s="18">
-        <v>29</v>
-      </c>
-      <c r="B57" s="9">
-        <v>44816.906886574099</v>
-      </c>
-      <c r="C57" s="10" t="s">
-        <v>294</v>
-      </c>
-      <c r="D57" s="10" t="s">
-        <v>295</v>
-      </c>
-      <c r="E57" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F57" s="10" t="s">
-        <v>296</v>
-      </c>
-      <c r="G57" s="10" t="s">
-        <v>297</v>
-      </c>
-      <c r="H57" s="10" t="s">
-        <v>298</v>
-      </c>
-      <c r="I57" s="10" t="s">
-        <v>299</v>
-      </c>
-      <c r="J57" s="10" t="s">
-        <v>297</v>
-      </c>
-      <c r="K57" s="10" t="s">
-        <v>294</v>
-      </c>
-      <c r="L57" s="10" t="s">
-        <v>297</v>
-      </c>
-      <c r="M57" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="N57" s="10">
-        <v>29</v>
-      </c>
-      <c r="O57" s="10">
+      <c r="A57" s="19">
+        <v>39</v>
+      </c>
+      <c r="B57" s="20">
+        <v>44817.728460648199</v>
+      </c>
+      <c r="C57" s="21" t="s">
+        <v>357</v>
+      </c>
+      <c r="D57" s="21" t="s">
+        <v>358</v>
+      </c>
+      <c r="E57" s="21" t="s">
+        <v>359</v>
+      </c>
+      <c r="F57" s="21" t="s">
+        <v>360</v>
+      </c>
+      <c r="G57" s="21" t="s">
+        <v>361</v>
+      </c>
+      <c r="H57" s="21" t="s">
+        <v>362</v>
+      </c>
+      <c r="I57" s="21" t="s">
+        <v>363</v>
+      </c>
+      <c r="J57" s="21" t="s">
+        <v>364</v>
+      </c>
+      <c r="K57" s="21" t="s">
+        <v>361</v>
+      </c>
+      <c r="L57" s="21" t="s">
+        <v>357</v>
+      </c>
+      <c r="M57" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="N57" s="21">
+        <v>39</v>
+      </c>
+      <c r="O57" s="21">
         <f>MOD(N57,10)</f>
         <v>9</v>
       </c>
-      <c r="P57" s="8"/>
+      <c r="P57" s="8" t="s">
+        <v>457</v>
+      </c>
       <c r="Q57" s="8"/>
       <c r="R57" s="8"/>
     </row>
     <row r="58" spans="1:18" ht="18.75" customHeight="1">
-      <c r="B58" s="11"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
-      <c r="F58" s="8"/>
-      <c r="G58" s="8"/>
-      <c r="H58" s="8"/>
-      <c r="I58" s="8"/>
-      <c r="J58" s="8"/>
-      <c r="K58" s="8"/>
-      <c r="L58" s="8"/>
-      <c r="M58" s="8"/>
-      <c r="N58" s="8"/>
-      <c r="O58" s="8"/>
-      <c r="P58" s="8"/>
+      <c r="A58" s="18">
+        <v>9</v>
+      </c>
+      <c r="B58" s="9">
+        <v>44816.901365740698</v>
+      </c>
+      <c r="C58" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="D58" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="E58" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="F58" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="G58" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="H58" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="I58" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="J58" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="K58" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="L58" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="M58" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="N58" s="21">
+        <v>9</v>
+      </c>
+      <c r="O58" s="21">
+        <f>MOD(N58,10)</f>
+        <v>9</v>
+      </c>
+      <c r="P58" s="24" t="s">
+        <v>457</v>
+      </c>
       <c r="Q58" s="8"/>
       <c r="R58" s="8"/>
     </row>
     <row r="59" spans="1:18" ht="18.75" customHeight="1">
-      <c r="B59" s="11"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="8"/>
-      <c r="E59" s="8"/>
-      <c r="F59" s="8"/>
-      <c r="G59" s="8"/>
-      <c r="H59" s="8"/>
-      <c r="I59" s="8"/>
-      <c r="J59" s="8"/>
-      <c r="K59" s="8"/>
-      <c r="L59" s="8"/>
-      <c r="M59" s="8"/>
-      <c r="N59" s="8"/>
-      <c r="O59" s="8"/>
-      <c r="P59" s="8"/>
+      <c r="A59" s="25">
+        <v>29</v>
+      </c>
+      <c r="B59" s="26">
+        <v>44816.906886574099</v>
+      </c>
+      <c r="C59" s="27" t="s">
+        <v>294</v>
+      </c>
+      <c r="D59" s="27" t="s">
+        <v>295</v>
+      </c>
+      <c r="E59" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="F59" s="27" t="s">
+        <v>296</v>
+      </c>
+      <c r="G59" s="27" t="s">
+        <v>297</v>
+      </c>
+      <c r="H59" s="27" t="s">
+        <v>298</v>
+      </c>
+      <c r="I59" s="27" t="s">
+        <v>299</v>
+      </c>
+      <c r="J59" s="27" t="s">
+        <v>297</v>
+      </c>
+      <c r="K59" s="27" t="s">
+        <v>294</v>
+      </c>
+      <c r="L59" s="27" t="s">
+        <v>297</v>
+      </c>
+      <c r="M59" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="N59" s="21">
+        <v>29</v>
+      </c>
+      <c r="O59" s="21">
+        <f>MOD(N59,10)</f>
+        <v>9</v>
+      </c>
+      <c r="P59" s="8" t="s">
+        <v>457</v>
+      </c>
       <c r="Q59" s="8"/>
       <c r="R59" s="8"/>
     </row>
@@ -7187,9 +7378,10 @@
       <c r="R151" s="8"/>
     </row>
   </sheetData>
-  <sortState ref="A2:O57">
-    <sortCondition ref="O2:O57"/>
-    <sortCondition ref="D2:D57"/>
+  <sortState ref="A2:P59">
+    <sortCondition ref="O2:O59"/>
+    <sortCondition ref="D2:D59"/>
+    <sortCondition ref="P2:P59"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="C8" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>

</xml_diff>